<commit_message>
Merge merge-cosmo-in-dev in Cosmo OK!
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/Files/Cosmo/database_file_Cosmo.xlsx
+++ b/FlOpEDT/misc/deploy_database/Files/Cosmo/database_file_Cosmo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Intervenants" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,6 +13,7 @@
     <sheet name="Groupes" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Modules" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Cours" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Paramètres" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="154">
   <si>
     <t xml:space="preserve">Liste intervenants</t>
   </si>
@@ -68,9 +69,6 @@
     <t xml:space="preserve">Permanent</t>
   </si>
   <si>
-    <t xml:space="preserve">test@test.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adelaide</t>
   </si>
   <si>
@@ -110,6 +108,9 @@
     <t xml:space="preserve">Florian</t>
   </si>
   <si>
+    <t xml:space="preserve">Manon</t>
+  </si>
+  <si>
     <t xml:space="preserve">Liste Salles</t>
   </si>
   <si>
@@ -441,15 +442,61 @@
   </si>
   <si>
     <t xml:space="preserve">TP240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Horaires de fonctionnement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jours ouvrables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Début des cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lundi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mardi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercredi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jeudi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendredi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samedi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dimanche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin des cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Début de la pause déjeuner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin de la pause déjeuner</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="HH:MM"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -684,7 +731,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -845,6 +892,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -925,7 +988,7 @@
   <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="M20 A3"/>
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1010,8 +1073,9 @@
       <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
+      <c r="E3" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A3, "@american-cosmograph.fr")</f>
+        <v>Frederic@american-cosmograph.fr</v>
       </c>
       <c r="G3" s="9" t="str">
         <f aca="false">IF(Intervenants!D3="Vacataire",Intervenants!A3,"")</f>
@@ -1022,10 +1086,10 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>12</v>
@@ -1033,8 +1097,9 @@
       <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>14</v>
+      <c r="E4" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A4, "@american-cosmograph.fr")</f>
+        <v>Adelaide@american-cosmograph.fr</v>
       </c>
       <c r="G4" s="9" t="str">
         <f aca="false">IF(Intervenants!D4="Vacataire",Intervenants!A4,"")</f>
@@ -1045,10 +1110,10 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>12</v>
@@ -1056,8 +1121,9 @@
       <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
+      <c r="E5" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A5, "@american-cosmograph.fr")</f>
+        <v>Elsa@american-cosmograph.fr</v>
       </c>
       <c r="G5" s="9" t="str">
         <f aca="false">IF(Intervenants!D5="Vacataire",Intervenants!A5,"")</f>
@@ -1068,10 +1134,10 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>12</v>
@@ -1079,8 +1145,9 @@
       <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>14</v>
+      <c r="E6" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A6, "@american-cosmograph.fr")</f>
+        <v>Marine@american-cosmograph.fr</v>
       </c>
       <c r="G6" s="9" t="str">
         <f aca="false">IF(Intervenants!D6="Vacataire",Intervenants!A6,"")</f>
@@ -1091,10 +1158,10 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>12</v>
@@ -1102,8 +1169,9 @@
       <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>14</v>
+      <c r="E7" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A7, "@american-cosmograph.fr")</f>
+        <v>Emilie@american-cosmograph.fr</v>
       </c>
       <c r="G7" s="9" t="str">
         <f aca="false">IF(Intervenants!D7="Vacataire",Intervenants!A7,"")</f>
@@ -1114,10 +1182,10 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>12</v>
@@ -1125,8 +1193,9 @@
       <c r="D8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>14</v>
+      <c r="E8" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A8, "@american-cosmograph.fr")</f>
+        <v>Nicolas@american-cosmograph.fr</v>
       </c>
       <c r="G8" s="9" t="str">
         <f aca="false">IF(Intervenants!D8="Vacataire",Intervenants!A8,"")</f>
@@ -1137,10 +1206,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>12</v>
@@ -1148,8 +1217,9 @@
       <c r="D9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>14</v>
+      <c r="E9" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A9, "@american-cosmograph.fr")</f>
+        <v>Annie@american-cosmograph.fr</v>
       </c>
       <c r="G9" s="9" t="str">
         <f aca="false">IF(Intervenants!D9="Vacataire",Intervenants!A9,"")</f>
@@ -1160,10 +1230,10 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>22</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>23</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>12</v>
@@ -1171,8 +1241,9 @@
       <c r="D10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>14</v>
+      <c r="E10" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A10, "@american-cosmograph.fr")</f>
+        <v>Jeremy@american-cosmograph.fr</v>
       </c>
       <c r="G10" s="9" t="str">
         <f aca="false">IF(Intervenants!D10="Vacataire",Intervenants!A10,"")</f>
@@ -1183,10 +1254,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>12</v>
@@ -1194,8 +1265,9 @@
       <c r="D11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>14</v>
+      <c r="E11" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A11, "@american-cosmograph.fr")</f>
+        <v>Pierre@american-cosmograph.fr</v>
       </c>
       <c r="G11" s="9" t="str">
         <f aca="false">IF(Intervenants!D11="Vacataire",Intervenants!A11,"")</f>
@@ -1206,10 +1278,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>26</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>12</v>
@@ -1217,8 +1289,9 @@
       <c r="D12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>14</v>
+      <c r="E12" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A12, "@american-cosmograph.fr")</f>
+        <v>Leandre@american-cosmograph.fr</v>
       </c>
       <c r="G12" s="9" t="str">
         <f aca="false">IF(Intervenants!D12="Vacataire",Intervenants!A12,"")</f>
@@ -1229,10 +1302,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>12</v>
@@ -1240,8 +1313,9 @@
       <c r="D13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>14</v>
+      <c r="E13" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A13, "@american-cosmograph.fr")</f>
+        <v>Florian@american-cosmograph.fr</v>
       </c>
       <c r="G13" s="9" t="str">
         <f aca="false">IF(Intervenants!D13="Vacataire",Intervenants!A13,"")</f>
@@ -1251,11 +1325,22 @@
       <c r="I13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8" t="str">
+        <f aca="false">_xlfn.CONCAT(A14, "@american-cosmograph.fr")</f>
+        <v>Manon@american-cosmograph.fr</v>
+      </c>
       <c r="G14" s="9" t="str">
         <f aca="false">IF(Intervenants!D14="Vacataire",Intervenants!A14,"")</f>
         <v/>
@@ -2339,19 +2424,6 @@
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="test@test.com"/>
-    <hyperlink ref="E4" r:id="rId2" display="test@test.com"/>
-    <hyperlink ref="E5" r:id="rId3" display="test@test.com"/>
-    <hyperlink ref="E6" r:id="rId4" display="test@test.com"/>
-    <hyperlink ref="E7" r:id="rId5" display="test@test.com"/>
-    <hyperlink ref="E8" r:id="rId6" display="test@test.com"/>
-    <hyperlink ref="E9" r:id="rId7" display="test@test.com"/>
-    <hyperlink ref="E10" r:id="rId8" display="test@test.com"/>
-    <hyperlink ref="E11" r:id="rId9" display="test@test.com"/>
-    <hyperlink ref="E12" r:id="rId10" display="test@test.com"/>
-    <hyperlink ref="E13" r:id="rId11" display="test@test.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2370,7 +2442,7 @@
   <dimension ref="A1:T75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="1" sqref="M20 F22"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3314,7 +3386,7 @@
   </sheetPr>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M20" activeCellId="0" sqref="M20"/>
     </sheetView>
   </sheetViews>
@@ -3767,7 +3839,7 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="1" sqref="M20 C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3825,7 +3897,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>70</v>
@@ -3850,7 +3922,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="26" t="s">
         <v>70</v>
@@ -3875,7 +3947,7 @@
         <v>59</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="26" t="s">
         <v>70</v>
@@ -3895,7 +3967,7 @@
         <v>59</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="26" t="s">
         <v>70</v>
@@ -4402,7 +4474,7 @@
   <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="M20 E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5871,4 +5943,132 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.12"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="43" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="43" t="n">
+        <v>0.958333333333333</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="43" t="n">
+        <v>0.583333333333333</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="43" t="n">
+        <v>0.583333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:J1"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="true" showErrorMessage="true" showInputMessage="false" sqref="D2:J2" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>